<commit_message>
All test cases added 1-57
</commit_message>
<xml_diff>
--- a/Furniture_sale.xlsx
+++ b/Furniture_sale.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agil\TESTing Methoden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi_000\PycharmProjects\Furniture_sale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FD9B05-4A1D-462B-9FD0-E14EE787501D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDD1A03-8AF4-46C6-9F70-68FCB9D5359F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
   </bookViews>
   <sheets>
     <sheet name="calculate_discount_test" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
   <si>
     <t>ID</t>
   </si>
@@ -307,18 +307,6 @@
     <t>Discount 5% for total 90,00</t>
   </si>
   <si>
-    <t>Discount 10% for total 0,01</t>
-  </si>
-  <si>
-    <t>Discount 10% for total 99,99</t>
-  </si>
-  <si>
-    <t>Discount 10% for total 90,00</t>
-  </si>
-  <si>
-    <t>Discount 20% for total 0,01</t>
-  </si>
-  <si>
     <t>vEP1_2-BV1/vEP2_2</t>
   </si>
   <si>
@@ -358,9 +346,6 @@
     <t>vEP1_3-BV1/vEP2_3</t>
   </si>
   <si>
-    <t>vEP1_3-vEP/vEP2_3</t>
-  </si>
-  <si>
     <t>09.12.2022, first tier, maximum total</t>
   </si>
   <si>
@@ -514,9 +499,6 @@
     <t>Discount 5%+10% for total 99,99</t>
   </si>
   <si>
-    <t>Discount 10% +10% for total 100</t>
-  </si>
-  <si>
     <t>Discount 20%+10% for total 1000,00</t>
   </si>
   <si>
@@ -550,9 +532,6 @@
     <t>Discount 10% for total 499,999999. This number has to be truncated to 499,99</t>
   </si>
   <si>
-    <t>10% discount, truncation test</t>
-  </si>
-  <si>
     <t>Date 18.12.2022</t>
   </si>
   <si>
@@ -592,9 +571,6 @@
     <t>not a type of Date-2</t>
   </si>
   <si>
-    <t>88.13.9999</t>
-  </si>
-  <si>
     <t>negativ is not allowed</t>
   </si>
   <si>
@@ -671,14 +647,39 @@
   </si>
   <si>
     <t xml:space="preserve">Total number of testcases </t>
+  </si>
+  <si>
+    <t>vEP1_3-BV2/vEP2_3</t>
+  </si>
+  <si>
+    <t>10% discount, truncation test for value 499,999999</t>
+  </si>
+  <si>
+    <t>Discount 10% +10% for total 499.999999, this amount has to be trancated to 499.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not a type of Date-1year is wrong </t>
+  </si>
+  <si>
+    <t>not a type of Date-1,day is wrong</t>
+  </si>
+  <si>
+    <t>6.12.99999999999</t>
+  </si>
+  <si>
+    <t>88.12.2022</t>
+  </si>
+  <si>
+    <t>8.18.2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -872,12 +873,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -888,15 +898,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -906,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -986,19 +987,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1018,24 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1043,6 +1020,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,8 +1142,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFDAB449-FF4A-431B-AFF1-7BB1F03ADA86}" name="Tabelle2" displayName="Tabelle2" ref="A1:H64" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:H64" xr:uid="{AFDAB449-FF4A-431B-AFF1-7BB1F03ADA86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFDAB449-FF4A-431B-AFF1-7BB1F03ADA86}" name="Tabelle2" displayName="Tabelle2" ref="A1:H58" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A1:H58" xr:uid="{AFDAB449-FF4A-431B-AFF1-7BB1F03ADA86}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{84A6FB10-1051-4A26-AD9B-724C108FD978}" name="ID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{81809C38-79C8-484F-AB73-70648838E2A0}" name="Title" dataDxfId="6"/>
@@ -1448,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD5266E-D1D1-4282-9544-C85901BD3256}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,8 +1467,8 @@
     <col min="2" max="2" width="21.08984375" style="17" customWidth="1"/>
     <col min="3" max="3" width="28.90625" style="17" customWidth="1"/>
     <col min="4" max="4" width="19" style="17" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="17" customWidth="1"/>
     <col min="7" max="7" width="15.453125" style="17" customWidth="1"/>
     <col min="8" max="8" width="24.1796875" style="17" customWidth="1"/>
     <col min="9" max="16384" width="10.90625" style="17"/>
@@ -1548,7 +1555,7 @@
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
-        <f t="shared" ref="A4:A35" si="0">A3+1</f>
+        <f t="shared" ref="A4:A58" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -1627,40 +1634,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="31">
+    <row r="7" spans="1:8" s="32" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="50">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="32">
+      <c r="E7" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="33">
         <v>44890</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="32">
         <v>500</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="17">
+    <row r="8" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>85</v>
@@ -1682,12 +1689,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="17">
+      <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>88</v>
@@ -1709,12 +1716,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="17">
+      <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>89</v>
@@ -1736,18 +1743,18 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="17">
+      <c r="A11" s="21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>60</v>
@@ -1762,19 +1769,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="17">
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>60</v>
@@ -1782,26 +1789,26 @@
       <c r="F12" s="20">
         <v>44897</v>
       </c>
-      <c r="G12" s="17">
-        <v>499.99</v>
+      <c r="G12" s="52">
+        <v>499.999999</v>
       </c>
       <c r="H12" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="17">
+      <c r="A13" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>60</v>
@@ -1810,25 +1817,25 @@
         <v>44895</v>
       </c>
       <c r="G13" s="17">
-        <v>90</v>
+        <v>400</v>
       </c>
       <c r="H13" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
+      <c r="A14" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>60</v>
@@ -1844,1393 +1851,1231 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="17">
+      <c r="A15" s="21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="32">
+      <c r="D15" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="20">
+        <v>44897</v>
+      </c>
+      <c r="G15" s="17">
+        <v>999999.99</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="31">
         <v>44894</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G16" s="22">
         <v>10000</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H16" s="22">
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="17" t="s">
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="20">
-        <v>44893</v>
-      </c>
-      <c r="G16" s="17">
+      <c r="D17" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="20">
+        <v>44900</v>
+      </c>
+      <c r="G17" s="17">
         <v>0.01</v>
-      </c>
-      <c r="H16" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="20">
-        <v>44897</v>
-      </c>
-      <c r="G17" s="17">
-        <v>99.99</v>
       </c>
       <c r="H17" s="17">
         <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="17">
+      <c r="A18" s="21">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F18" s="20">
-        <v>44896</v>
+        <v>44902</v>
       </c>
       <c r="G18" s="17">
-        <v>90</v>
+        <v>99.99</v>
       </c>
       <c r="H18" s="17">
         <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="17">
+      <c r="A19" s="21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="20">
-        <v>44893</v>
+        <v>44901</v>
       </c>
       <c r="G19" s="17">
+        <v>90</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="20">
+        <v>44900</v>
+      </c>
+      <c r="G20" s="17">
         <v>100</v>
-      </c>
-      <c r="H19" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="17">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="20">
-        <v>44897</v>
-      </c>
-      <c r="G20" s="17">
-        <v>499.99</v>
       </c>
       <c r="H20" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="17">
+      <c r="A21" s="21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F21" s="20">
-        <v>44895</v>
-      </c>
-      <c r="G21" s="17">
-        <v>400</v>
+        <v>44902</v>
+      </c>
+      <c r="G21" s="52">
+        <v>499.999999</v>
       </c>
       <c r="H21" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="17">
+      <c r="A22" s="21">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F22" s="20">
-        <v>44893</v>
+        <v>44901</v>
       </c>
       <c r="G22" s="17">
+        <v>400</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="21">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="20">
+        <v>44900</v>
+      </c>
+      <c r="G23" s="17">
         <v>500</v>
-      </c>
-      <c r="H22" s="17">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="17">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="20">
-        <v>44897</v>
-      </c>
-      <c r="G23" s="17">
-        <v>999999.99</v>
       </c>
       <c r="H23" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="34">
+    <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="22">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="35">
-        <v>44894</v>
-      </c>
-      <c r="G24" s="34">
+      <c r="B24" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="31">
+        <v>44902</v>
+      </c>
+      <c r="G24" s="22">
         <v>10000</v>
       </c>
-      <c r="H24" s="34">
+      <c r="H24" s="22">
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17">
+    <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="21">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F25" s="20">
-        <v>44900</v>
+        <v>44904</v>
       </c>
       <c r="G25" s="17">
-        <v>0.01</v>
+        <v>99.99</v>
       </c>
       <c r="H25" s="17">
         <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="17">
+      <c r="A26" s="21">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="C26" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="20">
+        <v>44904</v>
+      </c>
+      <c r="G26" s="17">
+        <v>100</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="22" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="22">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="31">
+        <v>44904</v>
+      </c>
+      <c r="G27" s="22">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="20">
-        <v>44902</v>
-      </c>
-      <c r="G26" s="17">
+      <c r="D28" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="20">
+        <v>44907</v>
+      </c>
+      <c r="G28" s="17">
         <v>99.99</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H28" s="17">
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="17">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="20">
-        <v>44901</v>
-      </c>
-      <c r="G27" s="17">
-        <v>90</v>
-      </c>
-      <c r="H27" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="17">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="20">
-        <v>44900</v>
-      </c>
-      <c r="G28" s="17">
+    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="20">
+        <v>44911</v>
+      </c>
+      <c r="G29" s="17">
         <v>100</v>
-      </c>
-      <c r="H28" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="17">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="20">
-        <v>44902</v>
-      </c>
-      <c r="G29" s="17">
-        <v>499.99</v>
       </c>
       <c r="H29" s="17">
         <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="17">
+      <c r="A30" s="22">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="31">
+        <v>44908</v>
+      </c>
+      <c r="G30" s="22">
+        <v>1000</v>
+      </c>
+      <c r="H30" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="20">
+        <v>44914</v>
+      </c>
+      <c r="G31" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="20">
+        <v>44918</v>
+      </c>
+      <c r="G32" s="17">
+        <v>499.999999</v>
+      </c>
+      <c r="H32" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="32" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="22">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="33">
+        <v>44916</v>
+      </c>
+      <c r="G33" s="32">
+        <v>1000</v>
+      </c>
+      <c r="H33" s="32">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="21">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="20">
+        <v>44891</v>
+      </c>
+      <c r="G34" s="17">
+        <v>99.99</v>
+      </c>
+      <c r="H34" s="17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="21">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="20">
+        <v>44891</v>
+      </c>
+      <c r="G35" s="17">
+        <v>100</v>
+      </c>
+      <c r="H35" s="17">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="21">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="17" t="s">
+      <c r="C36" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="20">
-        <v>44901</v>
-      </c>
-      <c r="G30" s="17">
+      <c r="D36" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="29">
+        <v>44891</v>
+      </c>
+      <c r="G36" s="21">
+        <v>1000</v>
+      </c>
+      <c r="H36" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="21">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="20">
+        <v>44898</v>
+      </c>
+      <c r="G37" s="17">
+        <v>99.99</v>
+      </c>
+      <c r="H37" s="17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="21">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="20">
+        <v>44905</v>
+      </c>
+      <c r="G38" s="52">
+        <v>499.999999</v>
+      </c>
+      <c r="H38" s="17">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="21">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="29">
+        <v>44912</v>
+      </c>
+      <c r="G39" s="21">
+        <v>1000</v>
+      </c>
+      <c r="H39" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="32">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="33">
+        <v>44919</v>
+      </c>
+      <c r="G40" s="32">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="32">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="21">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="20">
+        <v>44922</v>
+      </c>
+      <c r="G41" s="17">
+        <v>90</v>
+      </c>
+      <c r="H41" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="21">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="20">
+        <v>44933</v>
+      </c>
+      <c r="G42" s="17">
         <v>400</v>
       </c>
-      <c r="H30" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="17">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="20">
-        <v>44900</v>
-      </c>
-      <c r="G31" s="17">
+      <c r="H42" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="32">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="33">
+        <v>44924</v>
+      </c>
+      <c r="G43" s="32">
         <v>500</v>
       </c>
-      <c r="H31" s="17">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="22">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="32">
-        <v>44901</v>
-      </c>
-      <c r="G32" s="22">
-        <v>10000</v>
-      </c>
-      <c r="H32" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="17">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="20">
-        <v>44904</v>
-      </c>
-      <c r="G33" s="17">
-        <v>99.99</v>
-      </c>
-      <c r="H33" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="17">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="20">
-        <v>44904</v>
-      </c>
-      <c r="G34" s="17">
+      <c r="H43" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="21">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="20">
+        <v>44892</v>
+      </c>
+      <c r="G44" s="17">
         <v>100</v>
       </c>
-      <c r="H34" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="34">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="35">
-        <v>44904</v>
-      </c>
-      <c r="G35" s="34">
-        <v>1000</v>
-      </c>
-      <c r="H35" s="34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17">
-        <f t="shared" ref="A36:A38" si="1">A35+1</f>
-        <v>35</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="20">
-        <v>44907</v>
-      </c>
-      <c r="G36" s="17">
-        <v>99.99</v>
-      </c>
-      <c r="H36" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="17">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F37" s="20">
-        <v>44911</v>
-      </c>
-      <c r="G37" s="17">
+      <c r="H44" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="21">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="20">
+        <v>44899</v>
+      </c>
+      <c r="G45" s="17">
         <v>100</v>
       </c>
-      <c r="H37" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="22">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="32">
-        <v>44908</v>
-      </c>
-      <c r="G38" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H38" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="17">
-        <f t="shared" ref="A39:A64" si="2">A38+1</f>
-        <v>38</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="20">
-        <v>44914</v>
-      </c>
-      <c r="G39" s="17">
-        <v>0.01</v>
-      </c>
-      <c r="H39" s="17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="17">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="17" t="s">
+      <c r="H45" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="21">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="20">
-        <v>44918</v>
-      </c>
-      <c r="G40" s="17">
-        <v>499.999999</v>
-      </c>
-      <c r="H40" s="17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="22">
-        <f>A40+1</f>
-        <v>40</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F41" s="32">
-        <v>44916</v>
-      </c>
-      <c r="G41" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H41" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="17">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="20">
-        <v>44891</v>
-      </c>
-      <c r="G42" s="17">
-        <v>99.99</v>
-      </c>
-      <c r="H42" s="17">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="17">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F43" s="20">
-        <v>44891</v>
-      </c>
-      <c r="G43" s="17">
-        <v>100</v>
-      </c>
-      <c r="H43" s="17">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="21">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="29">
-        <v>44891</v>
-      </c>
-      <c r="G44" s="21">
-        <v>1000</v>
-      </c>
-      <c r="H44" s="21">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="17">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="20">
-        <v>44898</v>
-      </c>
-      <c r="G45" s="17">
-        <v>99.99</v>
-      </c>
-      <c r="H45" s="17">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="17">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>152</v>
+      <c r="D46" s="37" t="s">
+        <v>11</v>
       </c>
       <c r="E46" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F46" s="20">
-        <v>44905</v>
+        <v>44903</v>
       </c>
       <c r="G46" s="17">
         <v>100</v>
       </c>
-      <c r="H46" s="17">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H46" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="29">
-        <v>44912</v>
-      </c>
-      <c r="G47" s="21">
-        <v>1000</v>
-      </c>
-      <c r="H47" s="21">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="34">
-        <f t="shared" si="2"/>
+      <c r="B47" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="20">
+        <v>44906</v>
+      </c>
+      <c r="G47" s="17">
+        <v>100</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="21">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="35">
-        <v>44919</v>
-      </c>
-      <c r="G48" s="34">
-        <v>1000</v>
-      </c>
-      <c r="H48" s="34">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17">
-        <f t="shared" si="2"/>
+      <c r="B48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="20">
+        <v>44913</v>
+      </c>
+      <c r="G48" s="17">
+        <v>100</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="21">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>204</v>
+        <v>173</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>11</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F49" s="20">
-        <v>44922</v>
+        <v>44920</v>
       </c>
       <c r="G49" s="17">
-        <v>90</v>
-      </c>
-      <c r="H49" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="17">
-        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="21">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>205</v>
+        <v>173</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>11</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F50" s="20">
-        <v>44933</v>
+        <v>44921</v>
       </c>
       <c r="G50" s="17">
-        <v>400</v>
-      </c>
-      <c r="H50" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="34">
-        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="21">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="34" t="s">
+      <c r="B51" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="G51" s="17">
+        <v>100</v>
+      </c>
+      <c r="H51" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D51" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F51" s="35">
-        <v>44924</v>
-      </c>
-      <c r="G51" s="34">
-        <v>500</v>
-      </c>
-      <c r="H51" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="44" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="17">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="52" spans="1:8" s="39" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="21">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F52" s="20">
-        <v>44892</v>
-      </c>
-      <c r="G52" s="17">
+      <c r="B52" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G52" s="39">
         <v>100</v>
       </c>
-      <c r="H52" s="17" t="s">
+      <c r="H52" s="39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="21">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="39" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="17">
-        <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="20">
-        <v>44899</v>
-      </c>
-      <c r="G53" s="17">
+      <c r="D53" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G53" s="39">
         <v>100</v>
       </c>
-      <c r="H53" s="17" t="s">
-        <v>174</v>
+      <c r="H53" s="39" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="17">
-        <f t="shared" si="2"/>
+      <c r="A54" s="21">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="39" t="s">
-        <v>11</v>
+      <c r="D54" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="E54" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F54" s="20">
-        <v>44903</v>
+      <c r="F54" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="G54" s="17">
         <v>100</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="17">
-        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="21">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" s="39" t="s">
-        <v>11</v>
+        <v>178</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>190</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F55" s="20">
-        <v>44906</v>
+        <v>44912</v>
       </c>
       <c r="G55" s="17">
-        <v>100</v>
+        <v>-10000</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="17">
-        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="21">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" s="39" t="s">
-        <v>11</v>
+        <v>179</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F56" s="20">
-        <v>44913</v>
+        <v>44914</v>
       </c>
       <c r="G56" s="17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="17">
-        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="21">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D57" s="39" t="s">
-        <v>11</v>
+        <v>183</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F57" s="20">
-        <v>44920</v>
-      </c>
-      <c r="G57" s="17">
-        <v>100</v>
+        <v>44915</v>
+      </c>
+      <c r="G57" s="35">
+        <v>10.1234567</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="17">
-        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="21">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" s="39" t="s">
-        <v>11</v>
+        <v>184</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F58" s="20">
-        <v>44921</v>
-      </c>
-      <c r="G58" s="17">
-        <v>100</v>
+        <v>44917</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>7</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" s="17">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="G59" s="17">
-        <v>100</v>
-      </c>
-      <c r="H59" s="17" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="17">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>184</v>
-      </c>
       <c r="C60" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G60" s="17">
-        <v>100</v>
-      </c>
-      <c r="H60" s="17" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" s="17">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" s="20">
-        <v>44912</v>
-      </c>
-      <c r="G61" s="17">
-        <v>-10000</v>
-      </c>
-      <c r="H61" s="17" t="s">
-        <v>174</v>
+      <c r="C61" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" s="17">
-        <f t="shared" si="2"/>
-        <v>61</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F62" s="20">
-        <v>44914</v>
-      </c>
-      <c r="G62" s="17">
-        <v>0</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>174</v>
+      <c r="C62" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="17">
-        <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F63" s="20">
-        <v>44915</v>
-      </c>
-      <c r="G63" s="37">
-        <v>10.1234567</v>
-      </c>
-      <c r="H63" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="17">
-        <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="B64" s="17" t="s">
+      <c r="C63" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="17" t="s">
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66" s="23" t="s">
         <v>193</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F64" s="20">
-        <v>44917</v>
-      </c>
-      <c r="G64" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C66" s="17" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C68" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="C69" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C71" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C72" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C73" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="C74" s="23" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3246,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E64B6B9-ADBF-4B1D-B7B6-80EE0B4335B7}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3290,11 +3135,11 @@
         <v>52</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3326,11 +3171,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="46"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="44" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3356,11 +3201,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
@@ -3384,11 +3229,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
@@ -3408,11 +3253,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
@@ -3436,11 +3281,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
@@ -3464,20 +3309,20 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="38" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="11" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H8" s="1">
         <v>5</v>
@@ -3490,11 +3335,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="42" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -3520,20 +3365,20 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>195</v>
-      </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49" t="s">
-        <v>194</v>
+      <c r="D10" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41" t="s">
+        <v>186</v>
       </c>
       <c r="H10" s="1">
         <v>7</v>
@@ -3544,7 +3389,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
@@ -3568,7 +3413,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
@@ -3592,7 +3437,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -3621,13 +3466,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
+    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="48"/>
       <c r="B14" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>42</v>
@@ -3635,7 +3480,7 @@
       <c r="E14" s="13">
         <v>100</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="34">
         <v>499.999999</v>
       </c>
       <c r="G14" s="13">
@@ -3650,7 +3495,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="15" t="s">
         <v>16</v>
       </c>
@@ -3678,7 +3523,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="46"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="16" t="s">
         <v>17</v>
       </c>
@@ -3704,7 +3549,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="47"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
@@ -3732,16 +3577,16 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="43"/>
     </row>
     <row r="20" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>